<commit_message>
Simply used the material info
</commit_message>
<xml_diff>
--- a/SteelCraft.xlsx
+++ b/SteelCraft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\JavaProjects\SteelCraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F5E800-11E7-45E1-9273-D67D61E02964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86330FED-7BBB-47B0-A171-57EE82088572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="5250" windowWidth="28800" windowHeight="15435" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="5250" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工艺路线" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="92">
   <si>
     <t>工序名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -439,6 +439,14 @@
 退火（慢加热保温慢冷却）韧性↑硬度↓细化晶粒便于切削加工
 正火（= =。我记得跟退火类似）更多生成奥氏体
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>含水坩埚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>含岩浆坩埚</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1507,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973FADAB-C2FD-44F5-AF60-7EE6571BB98D}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1560,41 +1568,57 @@
     </row>
     <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="B6" s="14">
-        <v>5</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B7" s="14">
-        <v>-10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B8" s="14">
-        <v>-20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="14">
-        <v>-30</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="14">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="14">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B12" s="14">
         <v>20</v>
       </c>
     </row>
@@ -1608,7 +1632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFDB12A-E623-4BBE-AEB3-A617304BFB80}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>

</xml_diff>